<commit_message>
remapping votes complete - working on user interface
</commit_message>
<xml_diff>
--- a/2024-results-adjusted.xlsx
+++ b/2024-results-adjusted.xlsx
@@ -7318,7 +7318,7 @@
   <cols>
     <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
@@ -30278,7 +30278,7 @@
         <f>AF227/N227</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75">
       <c r="A228" s="5" t="s">
         <v>875</v>
       </c>
@@ -39267,7 +39267,7 @@
         <f>AF316/N316</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="317" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="317" customHeight="1" ht="18.75">
       <c r="A317" s="5" t="s">
         <v>1174</v>
       </c>
@@ -48458,7 +48458,7 @@
         <f>AF407/N407</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="408" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="408" customHeight="1" ht="18.75">
       <c r="A408" s="5" t="s">
         <v>1490</v>
       </c>
@@ -56841,7 +56841,7 @@
         <f>AF490/N490</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="491" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="491" customHeight="1" ht="18.75">
       <c r="A491" s="5" t="s">
         <v>1751</v>
       </c>

</xml_diff>